<commit_message>
a small change on level1
</commit_message>
<xml_diff>
--- a/地图设计.xlsx
+++ b/地图设计.xlsx
@@ -51,8 +51,8 @@
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="_ \￥* #,##0_ ;_ \￥* \-#,##0_ ;_ \￥* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ \￥* #,##0.00_ ;_ \￥* \-#,##0.00_ ;_ \￥* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ \￥* #,##0.00_ ;_ \￥* \-#,##0.00_ ;_ \￥* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ \￥* #,##0_ ;_ \￥* \-#,##0_ ;_ \￥* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -78,11 +78,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -91,13 +90,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -119,22 +111,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -148,9 +133,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -165,6 +165,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -172,17 +186,10 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -194,14 +201,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -216,18 +216,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.8"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -246,43 +246,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -294,133 +414,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -525,6 +525,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -554,17 +569,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -577,19 +586,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -598,40 +598,40 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -640,112 +640,110 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1173,7 +1171,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
-      <c r="N2" s="14"/>
+      <c r="N2" s="12"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
@@ -1193,16 +1191,16 @@
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
-      <c r="N3" s="14"/>
+      <c r="N3" s="12"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
@@ -1222,18 +1220,18 @@
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9" t="s">
+      <c r="E4" s="7"/>
+      <c r="F4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="7"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
-      <c r="N4" s="14"/>
+      <c r="N4" s="12"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
@@ -1253,16 +1251,16 @@
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
-      <c r="N5" s="14"/>
+      <c r="N5" s="12"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
@@ -1290,10 +1288,10 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
-      <c r="M6" s="15" t="s">
+      <c r="M6" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="N6" s="16"/>
+      <c r="N6" s="14"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
@@ -1321,8 +1319,8 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="16"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="14"/>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
@@ -1350,8 +1348,8 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="16"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="14"/>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
@@ -1380,7 +1378,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
-      <c r="N9" s="14"/>
+      <c r="N9" s="12"/>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
@@ -1409,7 +1407,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
-      <c r="N10" s="14"/>
+      <c r="N10" s="12"/>
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
@@ -1438,7 +1436,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
-      <c r="N11" s="14"/>
+      <c r="N11" s="12"/>
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
@@ -1467,7 +1465,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
-      <c r="N12" s="14"/>
+      <c r="N12" s="12"/>
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
@@ -1494,7 +1492,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
-      <c r="N13" s="14"/>
+      <c r="N13" s="12"/>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
@@ -1504,7 +1502,7 @@
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
-      <c r="Y13" s="13" t="s">
+      <c r="Y13" s="11" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1520,7 +1518,7 @@
   <dimension ref="A1:AA13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y6" sqref="Y6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1631,9 +1629,9 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
       <c r="W2" s="2"/>
@@ -1659,16 +1657,16 @@
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
-      <c r="Q3" s="10" t="s">
+      <c r="Q3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="R3" s="11" t="s">
+      <c r="R3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="S3" s="12" t="s">
+      <c r="S3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="T3" s="9"/>
+      <c r="T3" s="7"/>
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
@@ -1695,9 +1693,9 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="9"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
       <c r="W4" s="2"/>
@@ -1709,262 +1707,262 @@
         <v>3</v>
       </c>
       <c r="B5" s="4"/>
-      <c r="C5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="6"/>
-      <c r="U5" s="6"/>
-      <c r="V5" s="6"/>
-      <c r="W5" s="6"/>
-      <c r="X5" s="6"/>
-      <c r="Y5" s="6"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
     </row>
     <row r="6" ht="30" customHeight="1" spans="1:25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7"/>
-      <c r="U6" s="7"/>
-      <c r="V6" s="7"/>
-      <c r="W6" s="7"/>
-      <c r="X6" s="7"/>
-      <c r="Y6" s="7"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5"/>
     </row>
     <row r="7" ht="30" customHeight="1" spans="1:25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7"/>
-      <c r="U7" s="7"/>
-      <c r="V7" s="7"/>
-      <c r="W7" s="7"/>
-      <c r="X7" s="7"/>
-      <c r="Y7" s="7"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
     </row>
     <row r="8" ht="30" customHeight="1" spans="1:25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
-      <c r="U8" s="7"/>
-      <c r="V8" s="7"/>
-      <c r="W8" s="7"/>
-      <c r="X8" s="7"/>
-      <c r="Y8" s="7"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="5"/>
     </row>
     <row r="9" ht="30" customHeight="1" spans="1:25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="7"/>
-      <c r="U9" s="7"/>
-      <c r="V9" s="7"/>
-      <c r="W9" s="7"/>
-      <c r="X9" s="7"/>
-      <c r="Y9" s="7"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="5"/>
     </row>
     <row r="10" ht="30" customHeight="1" spans="1:25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
-      <c r="T10" s="7"/>
-      <c r="U10" s="7"/>
-      <c r="V10" s="7"/>
-      <c r="W10" s="7"/>
-      <c r="X10" s="7"/>
-      <c r="Y10" s="7"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="5"/>
     </row>
     <row r="11" ht="30" customHeight="1" spans="1:25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
-      <c r="S11" s="7"/>
-      <c r="T11" s="7"/>
-      <c r="U11" s="7"/>
-      <c r="V11" s="7"/>
-      <c r="W11" s="7"/>
-      <c r="X11" s="7"/>
-      <c r="Y11" s="7"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5"/>
     </row>
     <row r="12" ht="30" customHeight="1" spans="1:23">
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
-      <c r="S12" s="7"/>
-      <c r="T12" s="7"/>
-      <c r="U12" s="7"/>
-      <c r="V12" s="7"/>
-      <c r="W12" s="7"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
+      <c r="W12" s="5"/>
     </row>
     <row r="13" ht="30" customHeight="1" spans="1:25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="7"/>
-      <c r="S13" s="7"/>
-      <c r="T13" s="7"/>
-      <c r="U13" s="7"/>
-      <c r="V13" s="7"/>
-      <c r="W13" s="7"/>
-      <c r="Y13" s="13" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="5"/>
+      <c r="Y13" s="11" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
full loaded music effect
</commit_message>
<xml_diff>
--- a/地图设计.xlsx
+++ b/地图设计.xlsx
@@ -19,9 +19,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+  <si>
+    <t>主角</t>
+  </si>
+  <si>
+    <t>门</t>
+  </si>
   <si>
     <t>卷轴</t>
+  </si>
+  <si>
+    <t>通关点</t>
+  </si>
+  <si>
+    <t>教程顺序</t>
+  </si>
+  <si>
+    <t>演奏</t>
+  </si>
+  <si>
+    <t>行走</t>
+  </si>
+  <si>
+    <t>撞墙</t>
+  </si>
+  <si>
+    <t>门前弹音乐</t>
+  </si>
+  <si>
+    <t>找到卷轴</t>
+  </si>
+  <si>
+    <t>听卷轴</t>
+  </si>
+  <si>
+    <t>过关</t>
   </si>
   <si>
     <t>魔法门</t>
@@ -40,9 +73,6 @@
   </si>
   <si>
     <t>领舞小精灵</t>
-  </si>
-  <si>
-    <t>主角</t>
   </si>
   <si>
     <t>lover</t>
@@ -70,9 +100,6 @@
   </si>
   <si>
     <t>只有一条通路</t>
-  </si>
-  <si>
-    <t>门</t>
   </si>
   <si>
     <t>listening</t>
@@ -107,10 +134,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ \￥* #,##0.00_ ;_ \￥* \-#,##0.00_ ;_ \￥* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ \￥* #,##0_ ;_ \￥* \-#,##0_ ;_ \￥* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="_ \￥* #,##0_ ;_ \￥* \-#,##0_ ;_ \￥* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ \￥* #,##0.00_ ;_ \￥* \-#,##0.00_ ;_ \￥* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -124,6 +151,28 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -141,40 +190,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -187,28 +207,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -216,8 +214,16 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -225,9 +231,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -247,7 +253,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -256,22 +261,44 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="44">
+  <fills count="42">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -316,18 +343,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.6"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -352,7 +367,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -364,43 +487,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -412,43 +517,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -466,72 +541,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -621,34 +636,10 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color auto="1"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -669,11 +660,42 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -693,6 +715,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -707,19 +740,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -728,143 +752,143 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="39" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="39" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -877,24 +901,21 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1214,10 +1235,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Y13"/>
+  <dimension ref="A1:Y20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1304,349 +1325,394 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="12"/>
-      <c r="X2" s="12"/>
-      <c r="Y2" s="12"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
     </row>
     <row r="3" ht="30" customHeight="1" spans="1:25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="12"/>
-      <c r="U3" s="12"/>
-      <c r="V3" s="12"/>
-      <c r="W3" s="12"/>
-      <c r="X3" s="12"/>
-      <c r="Y3" s="12"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
     </row>
     <row r="4" ht="30" customHeight="1" spans="1:25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="12"/>
-      <c r="U4" s="12"/>
-      <c r="V4" s="12"/>
-      <c r="W4" s="12"/>
-      <c r="X4" s="12"/>
-      <c r="Y4" s="12"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
     </row>
     <row r="5" ht="30" customHeight="1" spans="1:25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="12"/>
-      <c r="S5" s="12"/>
-      <c r="T5" s="12"/>
-      <c r="U5" s="12"/>
-      <c r="V5" s="12"/>
-      <c r="W5" s="12"/>
-      <c r="X5" s="12"/>
-      <c r="Y5" s="12"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
     </row>
     <row r="6" ht="30" customHeight="1" spans="1:25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="12"/>
-      <c r="T6" s="12"/>
-      <c r="U6" s="12"/>
-      <c r="V6" s="12"/>
-      <c r="W6" s="12"/>
-      <c r="X6" s="12"/>
-      <c r="Y6" s="12"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="18"/>
+      <c r="T6" s="18"/>
+      <c r="U6" s="18"/>
+      <c r="V6" s="18"/>
+      <c r="W6" s="18"/>
+      <c r="X6" s="18"/>
+      <c r="Y6" s="18"/>
     </row>
     <row r="7" ht="30" customHeight="1" spans="1:25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="12"/>
-      <c r="S7" s="12"/>
-      <c r="T7" s="12"/>
-      <c r="U7" s="12"/>
-      <c r="V7" s="12"/>
-      <c r="W7" s="12"/>
-      <c r="X7" s="12"/>
-      <c r="Y7" s="12"/>
+      <c r="B7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
     </row>
     <row r="8" ht="30" customHeight="1" spans="1:25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="12"/>
-      <c r="S8" s="12"/>
-      <c r="T8" s="12"/>
-      <c r="U8" s="12"/>
-      <c r="V8" s="12"/>
-      <c r="W8" s="12"/>
-      <c r="X8" s="12"/>
-      <c r="Y8" s="12"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" ht="30" customHeight="1" spans="1:25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="12"/>
-      <c r="R9" s="12"/>
-      <c r="S9" s="12"/>
-      <c r="T9" s="12"/>
-      <c r="U9" s="12"/>
-      <c r="V9" s="12"/>
-      <c r="W9" s="12"/>
-      <c r="X9" s="12"/>
-      <c r="Y9" s="12"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="26"/>
+      <c r="O9" s="26"/>
+      <c r="P9" s="26"/>
+      <c r="Q9" s="26"/>
+      <c r="R9" s="26"/>
+      <c r="S9" s="26"/>
+      <c r="T9" s="26"/>
+      <c r="U9" s="26"/>
+      <c r="V9" s="26"/>
+      <c r="W9" s="26"/>
+      <c r="X9" s="26"/>
+      <c r="Y9" s="26"/>
     </row>
     <row r="10" ht="30" customHeight="1" spans="1:25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="12"/>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="12"/>
-      <c r="S10" s="12"/>
-      <c r="T10" s="12"/>
-      <c r="U10" s="12"/>
-      <c r="V10" s="12"/>
-      <c r="W10" s="12"/>
-      <c r="X10" s="12"/>
-      <c r="Y10" s="12"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
     </row>
     <row r="11" ht="30" customHeight="1" spans="1:25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="12"/>
-      <c r="Q11" s="12"/>
-      <c r="R11" s="12"/>
-      <c r="S11" s="12"/>
-      <c r="T11" s="12"/>
-      <c r="U11" s="12"/>
-      <c r="V11" s="12"/>
-      <c r="W11" s="12"/>
-      <c r="X11" s="12"/>
-      <c r="Y11" s="12"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
     </row>
     <row r="12" ht="30" customHeight="1" spans="1:25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="12"/>
-      <c r="Q12" s="12"/>
-      <c r="R12" s="12"/>
-      <c r="S12" s="12"/>
-      <c r="T12" s="12"/>
-      <c r="U12" s="12"/>
-      <c r="V12" s="12"/>
-      <c r="W12" s="12"/>
-      <c r="X12" s="12"/>
-      <c r="Y12" s="12"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
     </row>
     <row r="13" ht="30" customHeight="1" spans="1:25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="12"/>
-      <c r="S13" s="12"/>
-      <c r="T13" s="12"/>
-      <c r="U13" s="12"/>
-      <c r="V13" s="12"/>
-      <c r="W13" s="12"/>
-      <c r="X13" s="12"/>
-      <c r="Y13" s="13"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+    </row>
+    <row r="14" spans="9:9">
+      <c r="I14" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="9:9">
+      <c r="I15" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="9:9">
+      <c r="I16" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="9:9">
+      <c r="I17" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="9:9">
+      <c r="I18" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="9:9">
+      <c r="I19" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="9:9">
+      <c r="I20" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1759,7 +1825,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
-      <c r="N2" s="28"/>
+      <c r="N2" s="24"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
@@ -1788,7 +1854,7 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
-      <c r="N3" s="28"/>
+      <c r="N3" s="24"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
@@ -1810,7 +1876,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="2"/>
@@ -1819,7 +1885,7 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
-      <c r="N4" s="28"/>
+      <c r="N4" s="24"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
@@ -1848,7 +1914,7 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
-      <c r="N5" s="28"/>
+      <c r="N5" s="24"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
@@ -1876,10 +1942,10 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
-      <c r="M6" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="N6" s="29"/>
+      <c r="M6" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="N6" s="25"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
@@ -1907,8 +1973,8 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="29"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="25"/>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
@@ -1936,8 +2002,8 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="29"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="25"/>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
@@ -1966,7 +2032,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
-      <c r="N9" s="28"/>
+      <c r="N9" s="24"/>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
@@ -1995,7 +2061,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
-      <c r="N10" s="28"/>
+      <c r="N10" s="24"/>
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
@@ -2024,7 +2090,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
-      <c r="N11" s="28"/>
+      <c r="N11" s="24"/>
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
@@ -2053,7 +2119,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
-      <c r="N12" s="28"/>
+      <c r="N12" s="24"/>
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
@@ -2080,7 +2146,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
-      <c r="N13" s="28"/>
+      <c r="N13" s="24"/>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
@@ -2091,7 +2157,7 @@
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
       <c r="Y13" s="11" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2195,376 +2261,376 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="12"/>
-      <c r="X2" s="12"/>
-      <c r="Y2" s="12"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
       <c r="AA2" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" ht="30" customHeight="1" spans="1:25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="16"/>
-      <c r="S3" s="16"/>
-      <c r="T3" s="16"/>
-      <c r="U3" s="16"/>
-      <c r="V3" s="16"/>
-      <c r="W3" s="12"/>
-      <c r="X3" s="12"/>
-      <c r="Y3" s="12"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="14"/>
+      <c r="T3" s="14"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="14"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
     </row>
     <row r="4" ht="30" customHeight="1" spans="1:25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
-      <c r="O4" s="27"/>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="16"/>
-      <c r="S4" s="16"/>
-      <c r="T4" s="16"/>
-      <c r="U4" s="16"/>
-      <c r="V4" s="16"/>
-      <c r="W4" s="12"/>
-      <c r="X4" s="12"/>
-      <c r="Y4" s="12"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="14"/>
+      <c r="V4" s="14"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
     </row>
     <row r="5" ht="30" customHeight="1" spans="1:25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="27"/>
-      <c r="M5" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="N5" s="27"/>
-      <c r="O5" s="27"/>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="16"/>
-      <c r="S5" s="16"/>
-      <c r="T5" s="16"/>
-      <c r="U5" s="16"/>
-      <c r="V5" s="16"/>
-      <c r="W5" s="12"/>
-      <c r="X5" s="12"/>
-      <c r="Y5" s="12"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="14"/>
+      <c r="U5" s="14"/>
+      <c r="V5" s="14"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
     </row>
     <row r="6" ht="30" customHeight="1" spans="1:25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="27"/>
-      <c r="N6" s="27"/>
-      <c r="O6" s="27"/>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="16"/>
-      <c r="S6" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="T6" s="16"/>
-      <c r="U6" s="16"/>
-      <c r="V6" s="16"/>
-      <c r="W6" s="12"/>
-      <c r="X6" s="12"/>
-      <c r="Y6" s="12"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="T6" s="14"/>
+      <c r="U6" s="14"/>
+      <c r="V6" s="14"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
     </row>
     <row r="7" ht="30" customHeight="1" spans="1:25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="27"/>
-      <c r="N7" s="27"/>
-      <c r="O7" s="27"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="16"/>
-      <c r="S7" s="16"/>
-      <c r="T7" s="16"/>
-      <c r="U7" s="16"/>
-      <c r="V7" s="16"/>
-      <c r="W7" s="12"/>
-      <c r="X7" s="12"/>
-      <c r="Y7" s="12"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="14"/>
+      <c r="U7" s="14"/>
+      <c r="V7" s="14"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
     </row>
     <row r="8" ht="30" customHeight="1" spans="1:25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="16"/>
-      <c r="S8" s="16"/>
-      <c r="T8" s="16"/>
-      <c r="U8" s="16"/>
-      <c r="V8" s="16"/>
-      <c r="W8" s="12"/>
-      <c r="X8" s="12"/>
-      <c r="Y8" s="12"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="14"/>
+      <c r="U8" s="14"/>
+      <c r="V8" s="14"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
     </row>
     <row r="9" ht="30" customHeight="1" spans="1:25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22"/>
-      <c r="O9" s="22"/>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="23"/>
-      <c r="R9" s="23"/>
-      <c r="S9" s="23"/>
-      <c r="T9" s="23"/>
-      <c r="U9" s="23"/>
-      <c r="V9" s="23"/>
-      <c r="W9" s="22"/>
-      <c r="X9" s="22"/>
-      <c r="Y9" s="22"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="19"/>
+      <c r="T9" s="19"/>
+      <c r="U9" s="19"/>
+      <c r="V9" s="19"/>
+      <c r="W9" s="18"/>
+      <c r="X9" s="18"/>
+      <c r="Y9" s="18"/>
     </row>
     <row r="10" ht="30" customHeight="1" spans="1:25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
-      <c r="N10" s="24"/>
-      <c r="O10" s="24"/>
-      <c r="P10" s="24"/>
-      <c r="Q10" s="24"/>
-      <c r="R10" s="24"/>
-      <c r="S10" s="24"/>
-      <c r="T10" s="24"/>
-      <c r="U10" s="24"/>
-      <c r="V10" s="24"/>
-      <c r="W10" s="24"/>
-      <c r="X10" s="24"/>
-      <c r="Y10" s="24"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="20"/>
+      <c r="T10" s="20"/>
+      <c r="U10" s="20"/>
+      <c r="V10" s="20"/>
+      <c r="W10" s="20"/>
+      <c r="X10" s="20"/>
+      <c r="Y10" s="20"/>
     </row>
     <row r="11" ht="30" customHeight="1" spans="1:25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
-      <c r="N11" s="24"/>
-      <c r="O11" s="24"/>
-      <c r="P11" s="24"/>
-      <c r="Q11" s="24"/>
-      <c r="R11" s="24"/>
-      <c r="S11" s="24"/>
-      <c r="T11" s="24"/>
-      <c r="U11" s="24"/>
-      <c r="V11" s="24"/>
-      <c r="W11" s="24"/>
-      <c r="X11" s="24"/>
-      <c r="Y11" s="24"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="20"/>
+      <c r="S11" s="20"/>
+      <c r="T11" s="20"/>
+      <c r="U11" s="20"/>
+      <c r="V11" s="20"/>
+      <c r="W11" s="20"/>
+      <c r="X11" s="20"/>
+      <c r="Y11" s="20"/>
     </row>
     <row r="12" ht="30" customHeight="1" spans="1:25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="12"/>
-      <c r="Q12" s="12"/>
-      <c r="R12" s="12"/>
-      <c r="S12" s="12"/>
-      <c r="T12" s="12"/>
-      <c r="U12" s="12"/>
-      <c r="V12" s="12"/>
-      <c r="W12" s="12"/>
-      <c r="X12" s="12"/>
-      <c r="Y12" s="12"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
     </row>
     <row r="13" ht="30" customHeight="1" spans="1:25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="25"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="12"/>
-      <c r="S13" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="T13" s="12"/>
-      <c r="U13" s="12"/>
-      <c r="V13" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="W13" s="12"/>
-      <c r="X13" s="12"/>
-      <c r="Y13" s="13"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="21"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2665,15 +2731,15 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
       <c r="K2" s="11"/>
       <c r="L2" s="11"/>
       <c r="M2" s="11"/>
@@ -2689,332 +2755,332 @@
       <c r="W2" s="11"/>
       <c r="X2" s="11"/>
       <c r="Y2" s="11" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" ht="30" customHeight="1" spans="1:25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
-      <c r="T3" s="13"/>
-      <c r="U3" s="21"/>
-      <c r="V3" s="21"/>
-      <c r="W3" s="21"/>
-      <c r="X3" s="21"/>
-      <c r="Y3" s="21"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="17"/>
+      <c r="V3" s="17"/>
+      <c r="W3" s="17"/>
+      <c r="X3" s="17"/>
+      <c r="Y3" s="17"/>
     </row>
     <row r="4" ht="30" customHeight="1" spans="1:25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
       <c r="G4" s="11"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="21"/>
-      <c r="V4" s="21"/>
-      <c r="W4" s="21"/>
-      <c r="X4" s="21"/>
-      <c r="Y4" s="21"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="17"/>
+      <c r="V4" s="17"/>
+      <c r="W4" s="17"/>
+      <c r="X4" s="17"/>
+      <c r="Y4" s="17"/>
     </row>
     <row r="5" ht="30" customHeight="1" spans="1:25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
       <c r="G5" s="11"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="16"/>
-      <c r="S5" s="16"/>
-      <c r="T5" s="16"/>
-      <c r="U5" s="13"/>
-      <c r="V5" s="13"/>
-      <c r="W5" s="12"/>
-      <c r="X5" s="12"/>
-      <c r="Y5" s="13"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="14"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
     </row>
     <row r="6" ht="30" customHeight="1" spans="1:25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
       <c r="G6" s="11"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="12"/>
-      <c r="T6" s="16"/>
-      <c r="U6" s="12"/>
-      <c r="V6" s="13"/>
-      <c r="W6" s="13"/>
-      <c r="X6" s="12"/>
-      <c r="Y6" s="13"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="14"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
     </row>
     <row r="7" ht="30" customHeight="1" spans="1:25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
       <c r="G7" s="11"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="N7" s="19"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N7" s="16"/>
       <c r="O7" s="11"/>
       <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
       <c r="R7" s="11"/>
-      <c r="S7" s="12"/>
-      <c r="T7" s="16"/>
-      <c r="U7" s="12"/>
-      <c r="V7" s="12"/>
-      <c r="W7" s="13"/>
-      <c r="X7" s="13"/>
-      <c r="Y7" s="13"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="14"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
     </row>
     <row r="8" ht="30" customHeight="1" spans="1:25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
       <c r="G8" s="11"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="O8" s="13"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="12"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
       <c r="R8" s="11"/>
-      <c r="S8" s="12"/>
-      <c r="T8" s="16"/>
-      <c r="U8" s="12"/>
-      <c r="V8" s="12"/>
-      <c r="W8" s="12"/>
-      <c r="X8" s="12"/>
-      <c r="Y8" s="12"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="14"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
     </row>
     <row r="9" ht="30" customHeight="1" spans="1:25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
       <c r="G9" s="11"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
       <c r="Q9" s="11"/>
       <c r="R9" s="11"/>
-      <c r="S9" s="12"/>
-      <c r="T9" s="16"/>
-      <c r="U9" s="12"/>
-      <c r="V9" s="12"/>
-      <c r="W9" s="13"/>
-      <c r="X9" s="12"/>
-      <c r="Y9" s="12"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="14"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
     </row>
     <row r="10" ht="30" customHeight="1" spans="1:25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
-      <c r="K10" s="20"/>
+      <c r="K10" s="11"/>
       <c r="L10" s="11"/>
       <c r="M10" s="11"/>
       <c r="N10" s="11"/>
       <c r="O10" s="11"/>
       <c r="P10" s="11"/>
       <c r="Q10" s="11"/>
-      <c r="R10" s="13"/>
-      <c r="S10" s="12"/>
-      <c r="T10" s="16"/>
-      <c r="U10" s="12"/>
-      <c r="V10" s="12"/>
-      <c r="W10" s="13"/>
-      <c r="X10" s="12"/>
-      <c r="Y10" s="12"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="14"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
     </row>
     <row r="11" ht="30" customHeight="1" spans="1:25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="12"/>
-      <c r="Q11" s="12"/>
-      <c r="R11" s="13"/>
-      <c r="S11" s="12"/>
-      <c r="T11" s="16"/>
-      <c r="U11" s="12"/>
-      <c r="V11" s="12"/>
-      <c r="W11" s="13"/>
-      <c r="X11" s="12"/>
-      <c r="Y11" s="12"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="14"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
     </row>
     <row r="12" ht="30" customHeight="1" spans="1:25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="16"/>
-      <c r="Q12" s="16"/>
-      <c r="R12" s="16"/>
-      <c r="S12" s="16"/>
-      <c r="T12" s="16"/>
-      <c r="U12" s="12"/>
-      <c r="V12" s="12"/>
-      <c r="W12" s="13"/>
-      <c r="X12" s="12"/>
-      <c r="Y12" s="12"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="14"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
     </row>
     <row r="13" ht="30" customHeight="1" spans="1:25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17"/>
-      <c r="O13" s="17"/>
-      <c r="P13" s="17"/>
-      <c r="Q13" s="21"/>
-      <c r="R13" s="21"/>
-      <c r="S13" s="21"/>
-      <c r="T13" s="21"/>
-      <c r="U13" s="21"/>
-      <c r="V13" s="21"/>
-      <c r="W13" s="21"/>
-      <c r="X13" s="12"/>
-      <c r="Y13" s="13"/>
+      <c r="B13" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="17"/>
+      <c r="S13" s="17"/>
+      <c r="T13" s="17"/>
+      <c r="U13" s="17"/>
+      <c r="V13" s="17"/>
+      <c r="W13" s="17"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3115,358 +3181,358 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="12"/>
-      <c r="X2" s="14"/>
-      <c r="Y2" s="12"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="2"/>
     </row>
     <row r="3" ht="30" customHeight="1" spans="1:25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="12"/>
-      <c r="U3" s="12"/>
-      <c r="V3" s="12"/>
-      <c r="W3" s="12"/>
-      <c r="X3" s="14"/>
-      <c r="Y3" s="12"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="12"/>
+      <c r="Y3" s="2"/>
     </row>
     <row r="4" ht="30" customHeight="1" spans="1:25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="12"/>
-      <c r="U4" s="12"/>
-      <c r="V4" s="12"/>
-      <c r="W4" s="12"/>
-      <c r="X4" s="14"/>
-      <c r="Y4" s="12"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="12"/>
+      <c r="Y4" s="2"/>
     </row>
     <row r="5" ht="30" customHeight="1" spans="1:25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="12"/>
-      <c r="S5" s="12"/>
-      <c r="T5" s="12"/>
-      <c r="U5" s="12"/>
-      <c r="V5" s="12"/>
-      <c r="W5" s="12"/>
-      <c r="X5" s="14"/>
-      <c r="Y5" s="12"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="12"/>
+      <c r="Y5" s="2"/>
     </row>
     <row r="6" ht="30" customHeight="1" spans="1:25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="12"/>
-      <c r="T6" s="12"/>
-      <c r="U6" s="12"/>
-      <c r="V6" s="12"/>
-      <c r="W6" s="12"/>
-      <c r="X6" s="14"/>
-      <c r="Y6" s="12"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="12"/>
+      <c r="Y6" s="2"/>
     </row>
     <row r="7" ht="30" customHeight="1" spans="1:26">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="12"/>
-      <c r="S7" s="12"/>
-      <c r="T7" s="12"/>
-      <c r="U7" s="12"/>
-      <c r="V7" s="12"/>
-      <c r="W7" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="X7" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y7" s="15" t="s">
-        <v>19</v>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="X7" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y7" s="13" t="s">
+        <v>28</v>
       </c>
       <c r="Z7" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" ht="30" customHeight="1" spans="1:25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="12"/>
-      <c r="S8" s="12"/>
-      <c r="T8" s="12"/>
-      <c r="U8" s="12"/>
-      <c r="V8" s="12"/>
-      <c r="W8" s="12"/>
-      <c r="X8" s="14"/>
-      <c r="Y8" s="12"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="12"/>
+      <c r="Y8" s="2"/>
     </row>
     <row r="9" ht="30" customHeight="1" spans="1:25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="12"/>
-      <c r="R9" s="12"/>
-      <c r="S9" s="12"/>
-      <c r="T9" s="12"/>
-      <c r="U9" s="12"/>
-      <c r="V9" s="12"/>
-      <c r="W9" s="12"/>
-      <c r="X9" s="14"/>
-      <c r="Y9" s="12"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="12"/>
+      <c r="Y9" s="2"/>
     </row>
     <row r="10" ht="30" customHeight="1" spans="1:25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="12"/>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="12"/>
-      <c r="S10" s="12"/>
-      <c r="T10" s="12"/>
-      <c r="U10" s="12"/>
-      <c r="V10" s="12"/>
-      <c r="W10" s="12"/>
-      <c r="X10" s="14"/>
-      <c r="Y10" s="12"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="12"/>
+      <c r="Y10" s="2"/>
     </row>
     <row r="11" ht="30" customHeight="1" spans="1:25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="12"/>
-      <c r="Q11" s="12"/>
-      <c r="R11" s="12"/>
-      <c r="S11" s="12"/>
-      <c r="T11" s="12"/>
-      <c r="U11" s="12"/>
-      <c r="V11" s="12"/>
-      <c r="W11" s="12"/>
-      <c r="X11" s="14"/>
-      <c r="Y11" s="12"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="12"/>
+      <c r="Y11" s="2"/>
     </row>
     <row r="12" ht="30" customHeight="1" spans="1:25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="12"/>
-      <c r="Q12" s="12"/>
-      <c r="R12" s="12"/>
-      <c r="S12" s="12"/>
-      <c r="T12" s="12"/>
-      <c r="U12" s="12"/>
-      <c r="V12" s="12"/>
-      <c r="W12" s="12"/>
-      <c r="X12" s="14"/>
-      <c r="Y12" s="12"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="12"/>
+      <c r="Y12" s="2"/>
     </row>
     <row r="13" ht="30" customHeight="1" spans="1:25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="12"/>
-      <c r="S13" s="12"/>
-      <c r="T13" s="12"/>
-      <c r="U13" s="12"/>
-      <c r="V13" s="12"/>
-      <c r="W13" s="12"/>
-      <c r="X13" s="14"/>
-      <c r="Y13" s="13"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="12"/>
+      <c r="Y13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3480,7 +3546,7 @@
   <dimension ref="A1:AA13"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -3568,7 +3634,7 @@
         <v>23</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" ht="30" customHeight="1" spans="1:27">
@@ -3600,7 +3666,7 @@
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
       <c r="AA2" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" ht="30" customHeight="1" spans="1:27">
@@ -3620,13 +3686,13 @@
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="8" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="R3" s="9" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="S3" s="10" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T3" s="7"/>
       <c r="U3" s="2"/>
@@ -3635,7 +3701,7 @@
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
       <c r="AA3" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" ht="30" customHeight="1" spans="1:25">
@@ -3699,7 +3765,7 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="6" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -3711,7 +3777,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
       <c r="M6" s="5" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
@@ -3925,7 +3991,7 @@
       <c r="V13" s="5"/>
       <c r="W13" s="5"/>
       <c r="Y13" s="11" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
basic level4 and pics
</commit_message>
<xml_diff>
--- a/地图设计.xlsx
+++ b/地图设计.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="17700" windowHeight="9264"/>
+    <workbookView windowWidth="17700" windowHeight="9264" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="level0 " sheetId="5" r:id="rId1"/>
@@ -154,23 +154,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -183,8 +168,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -199,7 +192,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -210,30 +218,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -261,25 +245,33 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -297,6 +289,14 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="42">
     <fill>
@@ -367,7 +367,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -379,7 +439,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -391,7 +523,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -403,150 +541,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -644,16 +644,23 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color auto="1"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -663,15 +670,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -700,6 +698,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -711,17 +733,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -743,7 +754,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -761,134 +772,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -916,6 +927,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1237,8 +1249,8 @@
   <sheetPr/>
   <dimension ref="A1:Y20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y7" sqref="Y7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1479,23 +1491,23 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2"/>
-      <c r="Y7" s="2"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="18"/>
+      <c r="R7" s="18"/>
+      <c r="S7" s="18"/>
+      <c r="T7" s="18"/>
+      <c r="U7" s="18"/>
+      <c r="V7" s="18"/>
+      <c r="W7" s="18"/>
+      <c r="X7" s="18"/>
+      <c r="Y7" s="18"/>
     </row>
     <row r="8" ht="30" customHeight="1" spans="1:25">
       <c r="A8" s="1">
@@ -1726,7 +1738,7 @@
   <dimension ref="A1:Y13"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U11" sqref="U11"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -3093,8 +3105,8 @@
   <sheetPr/>
   <dimension ref="A1:Z13"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AA7" sqref="AA7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y7" sqref="Y7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>

</xml_diff>